<commit_message>
take minimum in account
</commit_message>
<xml_diff>
--- a/assets/ods/global_revenue_template.xlsx
+++ b/assets/ods/global_revenue_template.xlsx
@@ -15,9 +15,14 @@
   <definedNames>
     <definedName function="false" hidden="false" name="CONTRIBUTION_DIFFUSEUR_AGESSA" vbProcedure="false">Feuil1!$C$15</definedName>
     <definedName function="false" hidden="false" name="CONTRIBUTION_RETRAITE" vbProcedure="false">Feuil1!$C$14</definedName>
+    <definedName function="false" hidden="false" name="DIFFERENCE_RECETTE_MINIMUM_GARANTI" vbProcedure="false">Feuil1!$G$13</definedName>
     <definedName function="false" hidden="false" name="DROIT_D_AUTEUR" vbProcedure="false">Feuil1!$C$13</definedName>
     <definedName function="false" hidden="false" name="GRATUIT" vbProcedure="false">Feuil1!$F1</definedName>
     <definedName function="false" hidden="false" name="LIGNE_APPLICABLE" vbProcedure="false">Feuil1!$B1</definedName>
+    <definedName function="false" hidden="false" name="MINIMUM_COMPAGNIE_PAR_REPRESENTATION" vbProcedure="false">Feuil1!$G$12</definedName>
+    <definedName function="false" hidden="false" name="MINIMUM_GARANTI_THEATRE_PAR_REPRESENTATION" vbProcedure="false">Feuil1!$G$10</definedName>
+    <definedName function="false" hidden="false" name="MINIMUM_GARANTI_TOTAL" vbProcedure="false">Feuil1!$G$11</definedName>
+    <definedName function="false" hidden="false" name="NOMBRE_REPRESENTATIONS" vbProcedure="false">Feuil1!$A$9:$A$9</definedName>
     <definedName function="false" hidden="false" name="PART_COMPAGNIE" vbProcedure="false">Feuil1!$F$16</definedName>
     <definedName function="false" hidden="false" name="PART_THEATRE" vbProcedure="false">Feuil1!$F$15</definedName>
     <definedName function="false" hidden="false" name="PAYANT" vbProcedure="false">Feuil1!$E1</definedName>
@@ -26,7 +31,9 @@
     <definedName function="false" hidden="false" name="RECETTE_HTVA" vbProcedure="false">Feuil1!$C$12</definedName>
     <definedName function="false" hidden="false" name="RECETTE_NETTE" vbProcedure="false">Feuil1!$C$17</definedName>
     <definedName function="false" hidden="false" name="TAXE_PARAFISCALE" vbProcedure="false">Feuil1!$C$16</definedName>
+    <definedName function="false" hidden="false" name="TOTAL_THEATRE" vbProcedure="false">Feuil1!$G$15</definedName>
     <definedName function="false" hidden="false" name="TVA" vbProcedure="false">Feuil1!$C$11</definedName>
+    <definedName function="false" hidden="false" name="TVA_DIFFERENCE_MINIMUM_GARANTI" vbProcedure="false">Feuil1!$G$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -38,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t xml:space="preserve">BORDEREAU DE RECETTE :</t>
   </si>
@@ -103,16 +110,19 @@
     <t xml:space="preserve">RECETTE BRUTE :</t>
   </si>
   <si>
+    <t xml:space="preserve">minimum garanti par rep :</t>
+  </si>
+  <si>
     <t xml:space="preserve">TVA 2,10 % :</t>
   </si>
   <si>
-    <t xml:space="preserve">minimum garanti :</t>
+    <t xml:space="preserve">minimum garanti total :</t>
   </si>
   <si>
     <t xml:space="preserve">RECETTE HTVA :</t>
   </si>
   <si>
-    <t xml:space="preserve">minimun garanti encaissé :</t>
+    <t xml:space="preserve">minimum compagnie par rep :</t>
   </si>
   <si>
     <t xml:space="preserve">Droits d'Auteur 12 % :</t>
@@ -271,13 +281,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF003366"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF008000"/>
@@ -287,6 +290,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF003366"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF003366"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -392,15 +402,15 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
+      <left/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
+      <left style="thin"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -455,7 +465,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -572,119 +582,115 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,16 +747,16 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.09"/>
   </cols>
@@ -880,7 +886,7 @@
         <v>45701</v>
       </c>
       <c r="C9" s="22" t="n">
-        <v>423</v>
+        <v>520</v>
       </c>
       <c r="D9" s="23" t="n">
         <f aca="false">PAYANT + GRATUIT</f>
@@ -901,217 +907,228 @@
       <c r="B10" s="26"/>
       <c r="C10" s="27" t="n">
         <f aca="false">SUM(RECETTES)</f>
-        <v>423</v>
+        <v>520</v>
       </c>
       <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="G10" s="31" t="n">
+        <f aca="false">100</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33" t="n">
+      <c r="A11" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34" t="n">
         <f aca="false">(RECETTE_BRUTE-RECETTE_HTVA)</f>
-        <v>8.70029382957881</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35" t="s">
-        <v>22</v>
+        <v>10.6953966699314</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="F11" s="36"/>
+      <c r="G11" s="31" t="n">
+        <f aca="false">MINIMUM_GARANTI_THEATRE_PAR_REPRESENTATION*SUM(NOMBRE_REPRESENTATIONS)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33" t="n">
+        <v>24</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34" t="n">
         <f aca="false">(RECETTE_BRUTE/1.021)</f>
-        <v>414.299706170421</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35" t="s">
-        <v>24</v>
+        <v>509.304603330069</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="36"/>
-      <c r="G12" s="38" t="n">
-        <v>0</v>
+      <c r="G12" s="31" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="33" t="n">
+      <c r="B13" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="34" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",RECETTE_HTVA*0.12,0)</f>
-        <v>49.7159647404505</v>
-      </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="35" t="s">
+        <v>61.1165523996082</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="31" t="n">
+        <f aca="false">-MIN(RECETTE_NETTE - MINIMUM_GARANTI_TOTAL , 0)</f>
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="33" t="n">
+      <c r="C14" s="34" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",RECETTE_HTVA*0.01,0)</f>
-        <v>4.14299706170421</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="35" t="s">
-        <v>29</v>
+        <v>5.09304603330069</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="F14" s="36"/>
-      <c r="G14" s="38" t="n">
-        <v>0</v>
+      <c r="G14" s="31" t="n">
+        <f aca="false">0.2 * DIFFERENCE_RECETTE_MINIMUM_GARANTI</f>
+        <v>-0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="33" t="n">
+      <c r="A15" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="34" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",DROIT_D_AUTEUR * 0.01,0)</f>
-        <v>0.497159647404505</v>
-      </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="43" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G15" s="44" t="n">
-        <f aca="false">RECETTE_NETTE *PART_THEATRE</f>
-        <v>241.810166503428</v>
+        <v>0.611165523996082</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="43" t="n">
+        <f aca="false">MINIMUM_GARANTI_TOTAL + TVA_DIFFERENCE_MINIMUM_GARANTI + (RECETTE_NETTE - MIN(RECETTE_NETTE - MINIMUM_GARANTI_TOTAL, SUM(NOMBRE_REPRESENTATIONS) * MINIMUM_COMPAGNIE_PAR_REPRESENTATION)-MINIMUM_GARANTI_TOTAL) * PART_THEATRE</f>
+        <v>212.329089128306</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="33" t="n">
+      <c r="A16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="34" t="n">
         <f aca="false">(RECETTE_HTVA*0.035)</f>
-        <v>14.5004897159647</v>
-      </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="43" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="G16" s="47" t="n">
-        <f aca="false">RECETTE_NETTE*PART_COMPAGNIE</f>
-        <v>103.632928501469</v>
-      </c>
-      <c r="I16" s="48"/>
+        <v>17.8256611165524</v>
+      </c>
+      <c r="D16" s="35"/>
+      <c r="E16" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="46" t="n">
+        <f aca="false">RECETTE_NETTE - TOTAL_THEATRE</f>
+        <v>212.329089128306</v>
+      </c>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51" t="n">
+      <c r="A17" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50" t="n">
         <f aca="false">RECETTE_BRUTE - TVA-DROIT_D_AUTEUR - CONTRIBUTION_RETRAITE - CONTRIBUTION_DIFFUSEUR_AGESSA - TAXE_PARAFISCALE</f>
-        <v>345.443095004897</v>
-      </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
+        <v>424.658178256611</v>
+      </c>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" s="64" customFormat="true" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="60" t="s">
+    <row r="19" s="63" customFormat="true" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" s="64" customFormat="true" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="65" t="s">
+      <c r="B19" s="60"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="65" t="s">
+    </row>
+    <row r="20" s="63" customFormat="true" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="60" t="s">
+      <c r="B20" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="65"/>
-    </row>
-    <row r="21" s="64" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-    </row>
-    <row r="22" s="64" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C20" s="61"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="64"/>
+    </row>
+    <row r="21" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+    </row>
+    <row r="22" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-    </row>
-    <row r="23" s="64" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+    </row>
+    <row r="23" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-    </row>
-    <row r="24" s="64" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+    </row>
+    <row r="24" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
     </row>
     <row r="25" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1145,7 +1162,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1168,7 +1185,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix wrong management in case of negative company revenue
</commit_message>
<xml_diff>
--- a/assets/ods/global_revenue_template.xlsx
+++ b/assets/ods/global_revenue_template.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="CONTRIBUTION_DIFFUSEUR_AGESSA" vbProcedure="false">Feuil1!$C$15</definedName>
@@ -174,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="\ * #,##0.00\ [$€]\ ;\-* #,##0.00\ [$€]\ ;\ * \-#\ [$€]\ ;\ @\ "/>
     <numFmt numFmtId="166" formatCode="\ * #,##0.00\ [$€-1]\ ;\-* #,##0.00\ [$€-1]\ ;\ * \-#\ [$€-1]\ "/>
@@ -185,8 +185,9 @@
     <numFmt numFmtId="171" formatCode="\ * #,##0.00&quot; F &quot;;\-* #,##0.00&quot; F &quot;;\ * \-#&quot; F &quot;;\ @\ "/>
     <numFmt numFmtId="172" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="173" formatCode="0.00\ %"/>
-    <numFmt numFmtId="174" formatCode="\ * #,##0.00\ [$€-81D]\ ;\-* #,##0.00\ [$€-81D]\ ;\ * \-#\ [$€-81D]\ ;\ @\ "/>
-    <numFmt numFmtId="175" formatCode="\ * #,##0.00\ [$€-1]\ ;\-* #,##0.00\ [$€-1]\ ;\ * \-#\ [$€-1]\ ;\ @\ "/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ [$€-40C];[RED]\-#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="175" formatCode="\ * #,##0.00\ [$€-81D]\ ;\-* #,##0.00\ [$€-81D]\ ;\ * \-#\ [$€-81D]\ ;\ @\ "/>
+    <numFmt numFmtId="176" formatCode="\ * #,##0.00\ [$€-1]\ ;\-* #,##0.00\ [$€-1]\ ;\ * \-#\ [$€-1]\ ;\ @\ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -470,259 +471,259 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="18" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -739,277 +740,383 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="11" t="n">
         <v>45701</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="11" t="n">
         <v>45704</v>
       </c>
-      <c r="G5" s="11" t="n">
+      <c r="G5" s="12" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
+      <c r="A9" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="21" t="n">
+      <c r="B9" s="22" t="n">
         <v>45701</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="23" t="n">
         <v>520</v>
       </c>
-      <c r="D9" s="23" t="n">
+      <c r="D9" s="24" t="n">
         <f aca="false">PAYANT + GRATUIT</f>
         <v>27</v>
       </c>
-      <c r="E9" s="23" t="n">
+      <c r="E9" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="F9" s="24" t="n">
+      <c r="F9" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27" t="n">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28" t="n">
         <f aca="false">SUM(RECETTES)</f>
         <v>520</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31" t="n">
+      <c r="F10" s="31"/>
+      <c r="G10" s="32" t="n">
         <f aca="false">100</f>
         <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34" t="n">
+      <c r="B11" s="34"/>
+      <c r="C11" s="35" t="n">
         <f aca="false">(RECETTE_BRUTE-RECETTE_HTVA)</f>
         <v>10.6953966699314</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="29" t="s">
+      <c r="D11" s="36"/>
+      <c r="E11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="31" t="n">
+      <c r="F11" s="37"/>
+      <c r="G11" s="32" t="n">
         <f aca="false">MINIMUM_GARANTI_THEATRE_PAR_REPRESENTATION*SUM(NOMBRE_REPRESENTATIONS)</f>
         <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34" t="n">
+      <c r="B12" s="34"/>
+      <c r="C12" s="35" t="n">
         <f aca="false">(RECETTE_BRUTE/1.021)</f>
         <v>509.304603330069</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="29" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="31" t="n">
+      <c r="F12" s="37"/>
+      <c r="G12" s="32" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="34" t="n">
+      <c r="C13" s="35" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",RECETTE_HTVA*0.12,0)</f>
         <v>61.1165523996082</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="29" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="31" t="n">
+      <c r="F13" s="37"/>
+      <c r="G13" s="32" t="n">
         <f aca="false">-MIN(RECETTE_NETTE - MINIMUM_GARANTI_TOTAL , 0)</f>
         <v>-0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="34" t="n">
+      <c r="C14" s="35" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",RECETTE_HTVA*0.01,0)</f>
         <v>5.09304603330069</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="36"/>
+      <c r="E14" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="31" t="n">
+      <c r="F14" s="37"/>
+      <c r="G14" s="32" t="n">
         <f aca="false">0.2 * DIFFERENCE_RECETTE_MINIMUM_GARANTI</f>
         <v>-0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="34" t="n">
+      <c r="C15" s="35" t="n">
         <f aca="false">IF(LIGNE_APPLICABLE="Applicable",DROIT_D_AUTEUR * 0.01,0)</f>
         <v>0.611165523996082</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="41" t="s">
         <v>32</v>
       </c>
@@ -1022,15 +1129,15 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="44"/>
-      <c r="C16" s="34" t="n">
+      <c r="C16" s="35" t="n">
         <f aca="false">(RECETTE_HTVA*0.035)</f>
         <v>17.8256611165524</v>
       </c>
-      <c r="D16" s="35"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="45" t="s">
         <v>34</v>
       </c>
@@ -1063,8 +1170,8 @@
       <c r="C18" s="56"/>
       <c r="D18" s="57"/>
       <c r="E18" s="58"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" s="63" customFormat="true" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="59" t="s">
@@ -1104,29 +1211,29 @@
       <c r="G21" s="64"/>
     </row>
     <row r="22" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="64"/>
       <c r="G22" s="64"/>
     </row>
     <row r="23" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="64"/>
       <c r="G23" s="64"/>
     </row>
     <row r="24" s="63" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="64"/>
       <c r="G24" s="64"/>
     </row>
@@ -1152,7 +1259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1175,7 +1282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>

</xml_diff>